<commit_message>
removal of unused samples
</commit_message>
<xml_diff>
--- a/data_folder/Satlin individual n1 trimmed.xlsx
+++ b/data_folder/Satlin individual n1 trimmed.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t xml:space="preserve">strain</t>
   </si>
@@ -44,9 +44,6 @@
     <t xml:space="preserve">Negative</t>
   </si>
   <si>
-    <t xml:space="preserve">b5145</t>
-  </si>
-  <si>
     <t xml:space="preserve">b5146</t>
   </si>
   <si>
@@ -83,27 +80,18 @@
     <t xml:space="preserve">b5157</t>
   </si>
   <si>
-    <t xml:space="preserve">b5158</t>
-  </si>
-  <si>
     <t xml:space="preserve">b5159</t>
   </si>
   <si>
     <t xml:space="preserve">b5160</t>
   </si>
   <si>
-    <t xml:space="preserve">b5161</t>
-  </si>
-  <si>
     <t xml:space="preserve">b5162</t>
   </si>
   <si>
     <t xml:space="preserve">b5163</t>
   </si>
   <si>
-    <t xml:space="preserve">b5164</t>
-  </si>
-  <si>
     <t xml:space="preserve">b5165</t>
   </si>
   <si>
@@ -174,9 +162,6 @@
   </si>
   <si>
     <t xml:space="preserve">b5188</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b5189</t>
   </si>
   <si>
     <t xml:space="preserve">b5190</t>
@@ -654,16 +639,16 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -674,13 +659,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
@@ -691,13 +676,13 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -708,7 +693,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -722,16 +707,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
@@ -742,13 +727,13 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
@@ -759,13 +744,13 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
@@ -790,16 +775,16 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
@@ -807,16 +792,16 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
@@ -841,16 +826,16 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16">
@@ -858,16 +843,16 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
@@ -875,16 +860,16 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
@@ -892,16 +877,16 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19">
@@ -909,16 +894,16 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20">
@@ -926,16 +911,16 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21">
@@ -943,16 +928,16 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
@@ -960,16 +945,16 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
@@ -977,13 +962,13 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E23" t="s">
         <v>7</v>
@@ -994,16 +979,16 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
@@ -1011,16 +996,16 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26">
@@ -1034,10 +1019,10 @@
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
@@ -1045,10 +1030,10 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
@@ -1065,13 +1050,13 @@
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29">
@@ -1079,10 +1064,10 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
@@ -1096,7 +1081,7 @@
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
         <v>7</v>
@@ -1116,13 +1101,13 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32">
@@ -1130,10 +1115,10 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D32" t="s">
         <v>6</v>
@@ -1181,16 +1166,16 @@
         <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36">
@@ -1198,16 +1183,16 @@
         <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E36" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37">
@@ -1215,16 +1200,16 @@
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E37" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38">
@@ -1232,16 +1217,16 @@
         <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E38" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39">
@@ -1252,13 +1237,13 @@
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40">
@@ -1266,16 +1251,16 @@
         <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E40" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41">
@@ -1283,16 +1268,16 @@
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E41" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42">
@@ -1300,16 +1285,16 @@
         <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43">
@@ -1317,16 +1302,16 @@
         <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E43" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44">
@@ -1337,13 +1322,13 @@
         <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E44" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45">
@@ -1351,16 +1336,16 @@
         <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46">
@@ -1368,7 +1353,7 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
@@ -1391,10 +1376,10 @@
         <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48">
@@ -1402,16 +1387,16 @@
         <v>54</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D48" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E48" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49">
@@ -1419,16 +1404,16 @@
         <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E49" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50">
@@ -1436,10 +1421,10 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D50" t="s">
         <v>6</v>
@@ -1462,7 +1447,7 @@
         <v>6</v>
       </c>
       <c r="E51" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52">
@@ -1470,10 +1455,10 @@
         <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D52" t="s">
         <v>6</v>
@@ -1487,13 +1472,13 @@
         <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D53" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E53" t="s">
         <v>7</v>
@@ -1504,16 +1489,16 @@
         <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D54" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E54" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55">
@@ -1521,7 +1506,7 @@
         <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
         <v>7</v>
@@ -1538,7 +1523,7 @@
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
@@ -1547,7 +1532,7 @@
         <v>6</v>
       </c>
       <c r="E56" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57">
@@ -1555,16 +1540,16 @@
         <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D57" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E57" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58">
@@ -1606,7 +1591,7 @@
         <v>66</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C60" t="s">
         <v>7</v>
@@ -1623,7 +1608,7 @@
         <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C61" t="s">
         <v>7</v>
@@ -1640,16 +1625,16 @@
         <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C62" t="s">
         <v>7</v>
       </c>
       <c r="D62" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E62" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63">
@@ -1660,10 +1645,10 @@
         <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E63" t="s">
         <v>7</v>
@@ -1674,16 +1659,16 @@
         <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C64" t="s">
         <v>7</v>
       </c>
       <c r="D64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65">
@@ -1691,7 +1676,7 @@
         <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C65" t="s">
         <v>7</v>
@@ -1711,7 +1696,7 @@
         <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D66" t="s">
         <v>6</v>
@@ -1725,16 +1710,16 @@
         <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68">
@@ -1748,7 +1733,7 @@
         <v>7</v>
       </c>
       <c r="D68" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E68" t="s">
         <v>7</v>
@@ -1759,16 +1744,16 @@
         <v>75</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C69" t="s">
         <v>7</v>
       </c>
       <c r="D69" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E69" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70">
@@ -1776,16 +1761,16 @@
         <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C70" t="s">
         <v>7</v>
       </c>
       <c r="D70" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E70" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71">
@@ -1793,10 +1778,10 @@
         <v>77</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C71" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D71" t="s">
         <v>6</v>
@@ -1813,7 +1798,7 @@
         <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D72" t="s">
         <v>6</v>
@@ -1833,94 +1818,9 @@
         <v>7</v>
       </c>
       <c r="D73" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E73" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s">
-        <v>80</v>
-      </c>
-      <c r="B74" t="s">
-        <v>9</v>
-      </c>
-      <c r="C74" t="s">
-        <v>7</v>
-      </c>
-      <c r="D74" t="s">
-        <v>9</v>
-      </c>
-      <c r="E74" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s">
-        <v>81</v>
-      </c>
-      <c r="B75" t="s">
-        <v>6</v>
-      </c>
-      <c r="C75" t="s">
-        <v>7</v>
-      </c>
-      <c r="D75" t="s">
-        <v>7</v>
-      </c>
-      <c r="E75" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s">
-        <v>82</v>
-      </c>
-      <c r="B76" t="s">
-        <v>6</v>
-      </c>
-      <c r="C76" t="s">
-        <v>7</v>
-      </c>
-      <c r="D76" t="s">
-        <v>6</v>
-      </c>
-      <c r="E76" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="s">
-        <v>83</v>
-      </c>
-      <c r="B77" t="s">
-        <v>6</v>
-      </c>
-      <c r="C77" t="s">
-        <v>7</v>
-      </c>
-      <c r="D77" t="s">
-        <v>6</v>
-      </c>
-      <c r="E77" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="s">
-        <v>84</v>
-      </c>
-      <c r="B78" t="s">
-        <v>7</v>
-      </c>
-      <c r="C78" t="s">
-        <v>7</v>
-      </c>
-      <c r="D78" t="s">
-        <v>6</v>
-      </c>
-      <c r="E78" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>